<commit_message>
adding dataset of org_ministry
</commit_message>
<xml_diff>
--- a/y-Manipulated Tables/DataSet/Tables/ORGANIZATION.xlsx
+++ b/y-Manipulated Tables/DataSet/Tables/ORGANIZATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BDSM\CSE303-sec-03-Group-03\y-Manipulated Tables\DataSet\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4340AA0D-1791-4666-B403-A42889FF5C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6310DA2D-2D3E-445E-AA7E-BD6CFD3DA3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,7 +385,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>